<commit_message>
Added new qualitative code comparison graphs
</commit_message>
<xml_diff>
--- a/grp-edgelist.xlsx
+++ b/grp-edgelist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annie Armstrong\Documents\Github\mindmap\grp_edgelists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annie Armstrong\Documents\Github\mindmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C2F2E9-03D6-45E6-AD65-29DEF19F4A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16364317-7B83-4DEB-BA37-4DA46E958510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{AFA33BF0-5886-4B64-BE64-14EDB69C8799}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{AFA33BF0-5886-4B64-BE64-14EDB69C8799}"/>
   </bookViews>
   <sheets>
     <sheet name="Group list" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="427">
   <si>
     <t>Edge</t>
   </si>
@@ -818,9 +818,6 @@
     <t>Skill development</t>
   </si>
   <si>
-    <t>JOb</t>
-  </si>
-  <si>
     <t>River characteristics</t>
   </si>
   <si>
@@ -836,9 +833,6 @@
     <t>Teachers</t>
   </si>
   <si>
-    <t>SChool</t>
-  </si>
-  <si>
     <t>Bad</t>
   </si>
   <si>
@@ -1314,6 +1308,15 @@
   </si>
   <si>
     <t>QualitativeCode2</t>
+  </si>
+  <si>
+    <t>Environmental Action</t>
+  </si>
+  <si>
+    <t>Water Quality</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -1683,12 +1686,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75B9E74-F85C-4AA5-B2A7-0BAD20C99193}">
   <dimension ref="A1:H174"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E152" sqref="E152:E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="2" max="2" width="14.53125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1775,7 +1779,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>254</v>
@@ -1798,7 +1802,7 @@
         <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>254</v>
@@ -1887,7 +1891,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>70</v>
@@ -1956,10 +1960,10 @@
         <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>268</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>255</v>
@@ -1979,10 +1983,10 @@
         <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>268</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>255</v>
@@ -2002,7 +2006,7 @@
         <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>45</v>
@@ -2025,7 +2029,7 @@
         <v>35</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>46</v>
@@ -2048,7 +2052,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>38</v>
@@ -2071,7 +2075,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>156</v>
@@ -2097,7 +2101,7 @@
         <v>61</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>255</v>
@@ -2120,7 +2124,7 @@
         <v>61</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>255</v>
@@ -2143,7 +2147,7 @@
         <v>61</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>255</v>
@@ -2162,6 +2166,9 @@
       <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E21" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
@@ -2176,6 +2183,9 @@
       <c r="D22" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E22" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
@@ -2190,6 +2200,9 @@
       <c r="D23" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
@@ -2308,7 +2321,7 @@
         <v>56</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -2328,7 +2341,7 @@
         <v>56</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -2348,7 +2361,7 @@
         <v>61</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
@@ -2368,7 +2381,7 @@
         <v>61</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
@@ -2408,7 +2421,7 @@
         <v>65</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
@@ -2425,10 +2438,10 @@
         <v>35</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -2445,10 +2458,10 @@
         <v>35</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
@@ -2465,7 +2478,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>74</v>
@@ -2488,7 +2501,7 @@
         <v>35</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>15</v>
@@ -2626,7 +2639,7 @@
         <v>35</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>260</v>
+        <v>7</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>259</v>
@@ -2672,7 +2685,7 @@
         <v>35</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>260</v>
+        <v>7</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>259</v>
@@ -2695,13 +2708,13 @@
         <v>35</v>
       </c>
       <c r="E47" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="H47" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
@@ -2718,7 +2731,7 @@
         <v>35</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>16</v>
@@ -2779,7 +2792,7 @@
         <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
@@ -2816,10 +2829,10 @@
         <v>35</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>258</v>
+        <v>19</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
@@ -2836,10 +2849,10 @@
         <v>35</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>258</v>
+        <v>19</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
@@ -2856,7 +2869,7 @@
         <v>35</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>258</v>
+        <v>19</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>112</v>
@@ -2879,7 +2892,7 @@
         <v>166</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
@@ -2896,10 +2909,10 @@
         <v>35</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>266</v>
+        <v>166</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
@@ -2919,7 +2932,7 @@
         <v>166</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
@@ -2935,7 +2948,9 @@
       <c r="D59" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
@@ -2950,6 +2965,9 @@
       <c r="D60" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E60" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
@@ -2968,7 +2986,7 @@
         <v>19</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
@@ -3102,10 +3120,10 @@
         <v>98</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>254</v>
@@ -3125,7 +3143,7 @@
         <v>98</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>84</v>
@@ -3165,10 +3183,10 @@
         <v>98</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
@@ -3185,10 +3203,10 @@
         <v>98</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
@@ -3205,7 +3223,7 @@
         <v>98</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>256</v>
@@ -3225,7 +3243,7 @@
         <v>98</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>256</v>
@@ -3262,10 +3280,10 @@
         <v>98</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
@@ -3279,10 +3297,10 @@
         <v>98</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
@@ -3299,7 +3317,7 @@
         <v>98</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>55</v>
@@ -3458,7 +3476,7 @@
         <v>95</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
@@ -3518,7 +3536,7 @@
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
@@ -3534,6 +3552,9 @@
       <c r="D91" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="E91" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
@@ -3548,6 +3569,9 @@
       <c r="D92" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="E92" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
@@ -3562,6 +3586,9 @@
       <c r="D93" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="E93" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
@@ -3576,19 +3603,25 @@
       <c r="D94" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="E94" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>103</v>
       </c>
       <c r="B95" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>98</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
@@ -3596,7 +3629,7 @@
         <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>34</v>
@@ -3604,13 +3637,16 @@
       <c r="D96" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E96" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>34</v>
@@ -3618,8 +3654,11 @@
       <c r="D97" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E97" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -3632,8 +3671,11 @@
       <c r="D98" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E98" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -3646,8 +3688,11 @@
       <c r="D99" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E99" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>61</v>
       </c>
@@ -3660,8 +3705,11 @@
       <c r="D100" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E100" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>61</v>
       </c>
@@ -3674,8 +3722,11 @@
       <c r="D101" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E101" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>61</v>
       </c>
@@ -3688,8 +3739,11 @@
       <c r="D102" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E102" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>61</v>
       </c>
@@ -3702,8 +3756,11 @@
       <c r="D103" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E103" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>61</v>
       </c>
@@ -3716,13 +3773,16 @@
       <c r="D104" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E104" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>61</v>
       </c>
       <c r="B105" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>34</v>
@@ -3730,13 +3790,16 @@
       <c r="D105" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E105" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>61</v>
       </c>
       <c r="B106" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>34</v>
@@ -3744,13 +3807,16 @@
       <c r="D106" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E106" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>61</v>
       </c>
       <c r="B107" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>34</v>
@@ -3758,8 +3824,11 @@
       <c r="D107" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E107" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>61</v>
       </c>
@@ -3772,27 +3841,33 @@
       <c r="D108" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E108" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
+        <v>397</v>
+      </c>
+      <c r="B109" t="s">
         <v>399</v>
       </c>
-      <c r="B109" t="s">
-        <v>401</v>
-      </c>
       <c r="C109" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E109" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B110" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>34</v>
@@ -3800,13 +3875,16 @@
       <c r="D110" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E110" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>205</v>
       </c>
       <c r="B111" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>34</v>
@@ -3814,13 +3892,16 @@
       <c r="D111" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E111" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>205</v>
       </c>
       <c r="B112" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>34</v>
@@ -3828,13 +3909,16 @@
       <c r="D112" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E112" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>205</v>
       </c>
       <c r="B113" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>34</v>
@@ -3842,13 +3926,16 @@
       <c r="D113" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E113" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>205</v>
       </c>
       <c r="B114" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>34</v>
@@ -3856,13 +3943,16 @@
       <c r="D114" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E114" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>205</v>
       </c>
       <c r="B115" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>34</v>
@@ -3870,8 +3960,11 @@
       <c r="D115" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E115" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -3884,8 +3977,11 @@
       <c r="D116" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E116" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -3898,13 +3994,16 @@
       <c r="D117" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E117" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>90</v>
       </c>
       <c r="B118" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>34</v>
@@ -3912,13 +4011,16 @@
       <c r="D118" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E118" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>34</v>
@@ -3926,13 +4028,16 @@
       <c r="D119" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E119" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>90</v>
       </c>
       <c r="B120" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>34</v>
@@ -3940,13 +4045,16 @@
       <c r="D120" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E120" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>176</v>
       </c>
       <c r="B121" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>34</v>
@@ -3954,8 +4062,11 @@
       <c r="D121" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E121" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>176</v>
       </c>
@@ -3968,8 +4079,11 @@
       <c r="D122" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E122" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>176</v>
       </c>
@@ -3982,8 +4096,11 @@
       <c r="D123" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E123" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>176</v>
       </c>
@@ -3996,13 +4113,16 @@
       <c r="D124" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E124" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>176</v>
       </c>
       <c r="B125" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>34</v>
@@ -4010,13 +4130,16 @@
       <c r="D125" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E125" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>176</v>
       </c>
       <c r="B126" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>34</v>
@@ -4024,8 +4147,11 @@
       <c r="D126" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E126" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>49</v>
       </c>
@@ -4038,13 +4164,16 @@
       <c r="D127" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E127" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>49</v>
       </c>
       <c r="B128" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>34</v>
@@ -4052,8 +4181,11 @@
       <c r="D128" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E128" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>49</v>
       </c>
@@ -4066,8 +4198,11 @@
       <c r="D129" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E129" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>45</v>
       </c>
@@ -4080,13 +4215,16 @@
       <c r="D130" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E130" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>19</v>
       </c>
       <c r="B131" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>34</v>
@@ -4094,8 +4232,11 @@
       <c r="D131" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E131" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -4108,13 +4249,16 @@
       <c r="D132" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E132" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>19</v>
       </c>
       <c r="B133" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>34</v>
@@ -4122,13 +4266,16 @@
       <c r="D133" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E133" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B134" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>34</v>
@@ -4136,13 +4283,16 @@
       <c r="D134" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E134" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B135" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>34</v>
@@ -4150,13 +4300,16 @@
       <c r="D135" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E135" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>64</v>
       </c>
       <c r="B136" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>34</v>
@@ -4164,13 +4317,16 @@
       <c r="D136" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E136" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B137" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>34</v>
@@ -4178,10 +4334,13 @@
       <c r="D137" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E137" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B138" t="s">
         <v>228</v>
@@ -4192,36 +4351,45 @@
       <c r="D138" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E138" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
+        <v>410</v>
+      </c>
+      <c r="B139" t="s">
         <v>412</v>
       </c>
-      <c r="B139" t="s">
-        <v>414</v>
-      </c>
       <c r="C139" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E139" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
+        <v>411</v>
+      </c>
+      <c r="B140" t="s">
         <v>413</v>
       </c>
-      <c r="B140" t="s">
-        <v>415</v>
-      </c>
       <c r="C140" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E140" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>56</v>
       </c>
@@ -4234,8 +4402,11 @@
       <c r="D141" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E141" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>56</v>
       </c>
@@ -4248,13 +4419,16 @@
       <c r="D142" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E142" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>56</v>
       </c>
       <c r="B143" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>34</v>
@@ -4262,66 +4436,81 @@
       <c r="D143" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E143" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>96</v>
       </c>
       <c r="B144" t="s">
+        <v>414</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>399</v>
+      </c>
+      <c r="B145" t="s">
+        <v>400</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>394</v>
+      </c>
+      <c r="B146" t="s">
+        <v>351</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>415</v>
+      </c>
+      <c r="B147" t="s">
         <v>416</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A145" t="s">
-        <v>401</v>
-      </c>
-      <c r="B145" t="s">
-        <v>402</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A146" t="s">
-        <v>396</v>
-      </c>
-      <c r="B146" t="s">
-        <v>353</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
-        <v>417</v>
-      </c>
-      <c r="B147" t="s">
-        <v>418</v>
-      </c>
       <c r="C147" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E147" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B148" t="s">
         <v>55</v>
@@ -4332,55 +4521,67 @@
       <c r="D148" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E148" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B149" t="s">
+        <v>417</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>416</v>
+      </c>
+      <c r="B150" t="s">
+        <v>418</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>416</v>
+      </c>
+      <c r="B151" t="s">
         <v>419</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A150" t="s">
-        <v>418</v>
-      </c>
-      <c r="B150" t="s">
-        <v>420</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
-        <v>418</v>
-      </c>
-      <c r="B151" t="s">
-        <v>421</v>
-      </c>
       <c r="C151" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E151" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>55</v>
       </c>
       <c r="B152" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>34</v>
@@ -4388,13 +4589,16 @@
       <c r="D152" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E152" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>55</v>
       </c>
       <c r="B153" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>34</v>
@@ -4402,13 +4606,16 @@
       <c r="D153" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E153" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>55</v>
       </c>
       <c r="B154" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>34</v>
@@ -4416,13 +4623,16 @@
       <c r="D154" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E154" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>55</v>
       </c>
       <c r="B155" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>34</v>
@@ -4430,13 +4640,16 @@
       <c r="D155" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E155" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B156" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>34</v>
@@ -4445,12 +4658,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B157" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>34</v>
@@ -4459,12 +4672,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B158" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>34</v>
@@ -4473,12 +4686,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B159" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>34</v>
@@ -4487,12 +4700,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B160" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>34</v>
@@ -4506,7 +4719,7 @@
         <v>252</v>
       </c>
       <c r="B161" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>34</v>
@@ -4520,7 +4733,7 @@
         <v>252</v>
       </c>
       <c r="B162" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>34</v>
@@ -4531,10 +4744,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B163" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>34</v>
@@ -4548,7 +4761,7 @@
         <v>69</v>
       </c>
       <c r="B164" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>34</v>
@@ -4562,7 +4775,7 @@
         <v>69</v>
       </c>
       <c r="B165" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>34</v>
@@ -4576,7 +4789,7 @@
         <v>69</v>
       </c>
       <c r="B166" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>34</v>
@@ -4590,7 +4803,7 @@
         <v>69</v>
       </c>
       <c r="B167" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>34</v>
@@ -4604,7 +4817,7 @@
         <v>69</v>
       </c>
       <c r="B168" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>34</v>
@@ -4615,10 +4828,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B169" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>34</v>
@@ -4632,7 +4845,7 @@
         <v>256</v>
       </c>
       <c r="B170" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>34</v>
@@ -4646,7 +4859,7 @@
         <v>256</v>
       </c>
       <c r="B171" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>34</v>
@@ -4660,7 +4873,7 @@
         <v>12</v>
       </c>
       <c r="B172" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>34</v>
@@ -4674,7 +4887,7 @@
         <v>12</v>
       </c>
       <c r="B173" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>34</v>
@@ -4688,7 +4901,7 @@
         <v>12</v>
       </c>
       <c r="B174" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>34</v>
@@ -4708,7 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCFCEF4-088F-4F4C-BAD0-BADB2CC3EDCA}">
   <dimension ref="A1:Q354"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4737,10 +4950,10 @@
         <v>122</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>253</v>
@@ -5898,7 +6111,7 @@
         <v>121</v>
       </c>
       <c r="G48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
@@ -6103,7 +6316,7 @@
         <v>121</v>
       </c>
       <c r="G56" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -6558,7 +6771,7 @@
         <v>121</v>
       </c>
       <c r="G75" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
@@ -6639,7 +6852,7 @@
         <v>171</v>
       </c>
       <c r="I78" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
@@ -6662,10 +6875,10 @@
         <v>121</v>
       </c>
       <c r="G79" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I79" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
@@ -6688,7 +6901,7 @@
         <v>121</v>
       </c>
       <c r="G80" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I80" t="s">
         <v>254</v>
@@ -6858,7 +7071,7 @@
         <v>121</v>
       </c>
       <c r="G87" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
@@ -6881,7 +7094,7 @@
         <v>121</v>
       </c>
       <c r="G88" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I88" t="s">
         <v>254</v>
@@ -7198,7 +7411,7 @@
         <v>121</v>
       </c>
       <c r="G101" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
@@ -7221,7 +7434,7 @@
         <v>121</v>
       </c>
       <c r="G102" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I102" t="s">
         <v>255</v>
@@ -7408,7 +7621,7 @@
         <v>120</v>
       </c>
       <c r="G110" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I110" t="s">
         <v>255</v>
@@ -7705,7 +7918,7 @@
         <v>121</v>
       </c>
       <c r="G122" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I122" t="s">
         <v>254</v>
@@ -7731,7 +7944,7 @@
         <v>121</v>
       </c>
       <c r="G123" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I123" t="s">
         <v>255</v>
@@ -7757,7 +7970,7 @@
         <v>120</v>
       </c>
       <c r="G124" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I124" t="s">
         <v>255</v>
@@ -7783,7 +7996,7 @@
         <v>120</v>
       </c>
       <c r="G125" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I125" t="s">
         <v>255</v>
@@ -7809,7 +8022,7 @@
         <v>120</v>
       </c>
       <c r="G126" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I126" t="s">
         <v>255</v>
@@ -7835,7 +8048,7 @@
         <v>120</v>
       </c>
       <c r="G127" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I127" t="s">
         <v>255</v>
@@ -7864,7 +8077,7 @@
         <v>16</v>
       </c>
       <c r="H128" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.45">
@@ -7890,7 +8103,7 @@
         <v>16</v>
       </c>
       <c r="H129" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.45">
@@ -7916,7 +8129,7 @@
         <v>16</v>
       </c>
       <c r="H130" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.45">
@@ -7942,7 +8155,7 @@
         <v>16</v>
       </c>
       <c r="H131" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.45">
@@ -8423,7 +8636,7 @@
         <v>120</v>
       </c>
       <c r="G151" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.45">
@@ -8446,7 +8659,7 @@
         <v>120</v>
       </c>
       <c r="G152" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.45">
@@ -8541,7 +8754,7 @@
         <v>120</v>
       </c>
       <c r="G156" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.45">
@@ -8564,7 +8777,7 @@
         <v>120</v>
       </c>
       <c r="G157" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.45">
@@ -8607,7 +8820,7 @@
         <v>120</v>
       </c>
       <c r="G159" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I159" t="s">
         <v>255</v>
@@ -8633,7 +8846,7 @@
         <v>120</v>
       </c>
       <c r="G160" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I160" t="s">
         <v>255</v>
@@ -8659,7 +8872,7 @@
         <v>120</v>
       </c>
       <c r="G161" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I161" t="s">
         <v>255</v>
@@ -8685,7 +8898,7 @@
         <v>120</v>
       </c>
       <c r="G162" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I162" t="s">
         <v>255</v>
@@ -8737,7 +8950,7 @@
         <v>36</v>
       </c>
       <c r="I164" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.45">
@@ -8947,7 +9160,7 @@
         <v>98</v>
       </c>
       <c r="E173" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F173" t="s">
         <v>120</v>
@@ -8970,13 +9183,13 @@
         <v>98</v>
       </c>
       <c r="E174" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F174" t="s">
         <v>120</v>
       </c>
       <c r="G174" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.45">
@@ -8993,7 +9206,7 @@
         <v>98</v>
       </c>
       <c r="E175" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F175" t="s">
         <v>120</v>
@@ -9016,7 +9229,7 @@
         <v>98</v>
       </c>
       <c r="E176" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F176" t="s">
         <v>120</v>
@@ -9039,7 +9252,7 @@
         <v>98</v>
       </c>
       <c r="E177" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F177" t="s">
         <v>120</v>
@@ -9053,7 +9266,7 @@
         <v>45</v>
       </c>
       <c r="B178" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C178" t="s">
         <v>31</v>
@@ -9062,7 +9275,7 @@
         <v>98</v>
       </c>
       <c r="E178" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F178" t="s">
         <v>120</v>
@@ -9071,7 +9284,7 @@
         <v>19</v>
       </c>
       <c r="H178" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I178" t="s">
         <v>255</v>
@@ -9082,7 +9295,7 @@
         <v>45</v>
       </c>
       <c r="B179" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C179" t="s">
         <v>31</v>
@@ -9091,7 +9304,7 @@
         <v>98</v>
       </c>
       <c r="E179" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F179" t="s">
         <v>120</v>
@@ -9100,7 +9313,7 @@
         <v>19</v>
       </c>
       <c r="H179" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I179" t="s">
         <v>255</v>
@@ -9111,7 +9324,7 @@
         <v>45</v>
       </c>
       <c r="B180" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C180" t="s">
         <v>31</v>
@@ -9120,7 +9333,7 @@
         <v>98</v>
       </c>
       <c r="E180" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F180" t="s">
         <v>120</v>
@@ -9129,7 +9342,7 @@
         <v>19</v>
       </c>
       <c r="H180" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I180" t="s">
         <v>255</v>
@@ -9140,7 +9353,7 @@
         <v>45</v>
       </c>
       <c r="B181" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C181" t="s">
         <v>31</v>
@@ -9149,7 +9362,7 @@
         <v>98</v>
       </c>
       <c r="E181" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F181" t="s">
         <v>120</v>
@@ -9158,7 +9371,7 @@
         <v>19</v>
       </c>
       <c r="H181" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I181" t="s">
         <v>255</v>
@@ -9169,7 +9382,7 @@
         <v>45</v>
       </c>
       <c r="B182" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C182" t="s">
         <v>31</v>
@@ -9178,7 +9391,7 @@
         <v>98</v>
       </c>
       <c r="E182" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F182" t="s">
         <v>120</v>
@@ -9198,7 +9411,7 @@
         <v>45</v>
       </c>
       <c r="B183" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C183" t="s">
         <v>31</v>
@@ -9207,7 +9420,7 @@
         <v>98</v>
       </c>
       <c r="E183" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F183" t="s">
         <v>120</v>
@@ -9227,7 +9440,7 @@
         <v>45</v>
       </c>
       <c r="B184" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C184" t="s">
         <v>31</v>
@@ -9236,7 +9449,7 @@
         <v>98</v>
       </c>
       <c r="E184" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F184" t="s">
         <v>120</v>
@@ -9256,7 +9469,7 @@
         <v>45</v>
       </c>
       <c r="B185" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C185" t="s">
         <v>31</v>
@@ -9265,7 +9478,7 @@
         <v>98</v>
       </c>
       <c r="E185" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F185" t="s">
         <v>120</v>
@@ -9285,7 +9498,7 @@
         <v>45</v>
       </c>
       <c r="B186" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C186" t="s">
         <v>31</v>
@@ -9294,7 +9507,7 @@
         <v>98</v>
       </c>
       <c r="E186" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F186" t="s">
         <v>120</v>
@@ -9314,7 +9527,7 @@
         <v>45</v>
       </c>
       <c r="B187" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C187" t="s">
         <v>31</v>
@@ -9323,7 +9536,7 @@
         <v>98</v>
       </c>
       <c r="E187" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F187" t="s">
         <v>120</v>
@@ -9343,7 +9556,7 @@
         <v>45</v>
       </c>
       <c r="B188" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C188" t="s">
         <v>31</v>
@@ -9352,7 +9565,7 @@
         <v>98</v>
       </c>
       <c r="E188" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F188" t="s">
         <v>120</v>
@@ -9372,7 +9585,7 @@
         <v>45</v>
       </c>
       <c r="B189" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C189" t="s">
         <v>31</v>
@@ -9381,7 +9594,7 @@
         <v>98</v>
       </c>
       <c r="E189" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F189" t="s">
         <v>120</v>
@@ -9401,7 +9614,7 @@
         <v>129</v>
       </c>
       <c r="B190" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C190" t="s">
         <v>31</v>
@@ -9410,7 +9623,7 @@
         <v>98</v>
       </c>
       <c r="E190" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F190" t="s">
         <v>120</v>
@@ -9427,7 +9640,7 @@
         <v>129</v>
       </c>
       <c r="B191" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C191" t="s">
         <v>31</v>
@@ -9436,7 +9649,7 @@
         <v>98</v>
       </c>
       <c r="E191" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F191" t="s">
         <v>120</v>
@@ -9453,7 +9666,7 @@
         <v>129</v>
       </c>
       <c r="B192" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C192" t="s">
         <v>31</v>
@@ -9462,7 +9675,7 @@
         <v>98</v>
       </c>
       <c r="E192" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F192" t="s">
         <v>120</v>
@@ -9476,10 +9689,10 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B193" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C193" t="s">
         <v>31</v>
@@ -9488,7 +9701,7 @@
         <v>98</v>
       </c>
       <c r="E193" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F193" t="s">
         <v>120</v>
@@ -9505,7 +9718,7 @@
         <v>129</v>
       </c>
       <c r="B194" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C194" t="s">
         <v>31</v>
@@ -9514,7 +9727,7 @@
         <v>98</v>
       </c>
       <c r="E194" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F194" t="s">
         <v>120</v>
@@ -9528,7 +9741,7 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B195" t="s">
         <v>208</v>
@@ -9540,7 +9753,7 @@
         <v>98</v>
       </c>
       <c r="E195" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F195" t="s">
         <v>120</v>
@@ -9557,7 +9770,7 @@
         <v>123</v>
       </c>
       <c r="B196" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C196" t="s">
         <v>31</v>
@@ -9566,7 +9779,7 @@
         <v>98</v>
       </c>
       <c r="E196" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F196" t="s">
         <v>120</v>
@@ -9592,7 +9805,7 @@
         <v>98</v>
       </c>
       <c r="E197" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F197" t="s">
         <v>120</v>
@@ -9609,7 +9822,7 @@
         <v>123</v>
       </c>
       <c r="B198" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C198" t="s">
         <v>31</v>
@@ -9618,7 +9831,7 @@
         <v>98</v>
       </c>
       <c r="E198" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F198" t="s">
         <v>120</v>
@@ -9635,7 +9848,7 @@
         <v>67</v>
       </c>
       <c r="B199" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C199" t="s">
         <v>31</v>
@@ -9644,7 +9857,7 @@
         <v>98</v>
       </c>
       <c r="E199" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F199" t="s">
         <v>120</v>
@@ -9653,7 +9866,7 @@
         <v>67</v>
       </c>
       <c r="H199" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.45">
@@ -9661,7 +9874,7 @@
         <v>67</v>
       </c>
       <c r="B200" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C200" t="s">
         <v>31</v>
@@ -9670,7 +9883,7 @@
         <v>98</v>
       </c>
       <c r="E200" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F200" t="s">
         <v>120</v>
@@ -9679,7 +9892,7 @@
         <v>67</v>
       </c>
       <c r="H200" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.45">
@@ -9687,7 +9900,7 @@
         <v>67</v>
       </c>
       <c r="B201" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C201" t="s">
         <v>31</v>
@@ -9696,7 +9909,7 @@
         <v>98</v>
       </c>
       <c r="E201" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F201" t="s">
         <v>120</v>
@@ -9705,7 +9918,7 @@
         <v>67</v>
       </c>
       <c r="H201" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.45">
@@ -9713,7 +9926,7 @@
         <v>67</v>
       </c>
       <c r="B202" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C202" t="s">
         <v>31</v>
@@ -9722,13 +9935,13 @@
         <v>98</v>
       </c>
       <c r="E202" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F202" t="s">
         <v>120</v>
       </c>
       <c r="G202" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I202" t="s">
         <v>254</v>
@@ -9739,7 +9952,7 @@
         <v>67</v>
       </c>
       <c r="B203" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C203" t="s">
         <v>31</v>
@@ -9748,7 +9961,7 @@
         <v>98</v>
       </c>
       <c r="E203" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F203" t="s">
         <v>120</v>
@@ -9771,7 +9984,7 @@
         <v>98</v>
       </c>
       <c r="E204" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F204" t="s">
         <v>120</v>
@@ -9794,7 +10007,7 @@
         <v>98</v>
       </c>
       <c r="E205" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F205" t="s">
         <v>120</v>
@@ -9808,7 +10021,7 @@
         <v>12</v>
       </c>
       <c r="B206" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C206" t="s">
         <v>31</v>
@@ -9817,7 +10030,7 @@
         <v>98</v>
       </c>
       <c r="E206" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F206" t="s">
         <v>120</v>
@@ -9831,7 +10044,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C207" t="s">
         <v>31</v>
@@ -9840,13 +10053,13 @@
         <v>98</v>
       </c>
       <c r="E207" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F207" t="s">
         <v>120</v>
       </c>
       <c r="G207" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.45">
@@ -9854,7 +10067,7 @@
         <v>205</v>
       </c>
       <c r="B208" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C208" t="s">
         <v>31</v>
@@ -9863,13 +10076,13 @@
         <v>98</v>
       </c>
       <c r="E208" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F208" t="s">
         <v>120</v>
       </c>
       <c r="G208" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.45">
@@ -9877,7 +10090,7 @@
         <v>205</v>
       </c>
       <c r="B209" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C209" t="s">
         <v>31</v>
@@ -9886,13 +10099,13 @@
         <v>98</v>
       </c>
       <c r="E209" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F209" t="s">
         <v>120</v>
       </c>
       <c r="G209" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.45">
@@ -9900,7 +10113,7 @@
         <v>205</v>
       </c>
       <c r="B210" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C210" t="s">
         <v>31</v>
@@ -9909,13 +10122,13 @@
         <v>98</v>
       </c>
       <c r="E210" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F210" t="s">
         <v>120</v>
       </c>
       <c r="G210" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.45">
@@ -9923,7 +10136,7 @@
         <v>205</v>
       </c>
       <c r="B211" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C211" t="s">
         <v>31</v>
@@ -9932,13 +10145,13 @@
         <v>98</v>
       </c>
       <c r="E211" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F211" t="s">
         <v>120</v>
       </c>
       <c r="G211" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.45">
@@ -9946,7 +10159,7 @@
         <v>205</v>
       </c>
       <c r="B212" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C212" t="s">
         <v>31</v>
@@ -9955,13 +10168,13 @@
         <v>98</v>
       </c>
       <c r="E212" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F212" t="s">
         <v>120</v>
       </c>
       <c r="G212" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.45">
@@ -9978,7 +10191,7 @@
         <v>98</v>
       </c>
       <c r="E213" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F213" t="s">
         <v>120</v>
@@ -10001,7 +10214,7 @@
         <v>98</v>
       </c>
       <c r="E214" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F214" t="s">
         <v>120</v>
@@ -10024,7 +10237,7 @@
         <v>98</v>
       </c>
       <c r="E215" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F215" t="s">
         <v>120</v>
@@ -10047,7 +10260,7 @@
         <v>98</v>
       </c>
       <c r="E216" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F216" t="s">
         <v>120</v>
@@ -10070,7 +10283,7 @@
         <v>98</v>
       </c>
       <c r="E217" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F217" t="s">
         <v>120</v>
@@ -10093,7 +10306,7 @@
         <v>98</v>
       </c>
       <c r="E218" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F218" t="s">
         <v>120</v>
@@ -10116,7 +10329,7 @@
         <v>98</v>
       </c>
       <c r="E219" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F219" t="s">
         <v>120</v>
@@ -10139,7 +10352,7 @@
         <v>98</v>
       </c>
       <c r="E220" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F220" t="s">
         <v>120</v>
@@ -10162,7 +10375,7 @@
         <v>98</v>
       </c>
       <c r="E221" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F221" t="s">
         <v>120</v>
@@ -10176,16 +10389,16 @@
         <v>74</v>
       </c>
       <c r="B222" t="s">
+        <v>317</v>
+      </c>
+      <c r="C222" t="s">
+        <v>31</v>
+      </c>
+      <c r="D222" t="s">
+        <v>98</v>
+      </c>
+      <c r="E222" t="s">
         <v>319</v>
-      </c>
-      <c r="C222" t="s">
-        <v>31</v>
-      </c>
-      <c r="D222" t="s">
-        <v>98</v>
-      </c>
-      <c r="E222" t="s">
-        <v>321</v>
       </c>
       <c r="F222" t="s">
         <v>120</v>
@@ -10208,7 +10421,7 @@
         <v>98</v>
       </c>
       <c r="E223" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F223" t="s">
         <v>120</v>
@@ -10222,7 +10435,7 @@
         <v>74</v>
       </c>
       <c r="B224" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C224" t="s">
         <v>31</v>
@@ -10231,7 +10444,7 @@
         <v>98</v>
       </c>
       <c r="E224" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F224" t="s">
         <v>120</v>
@@ -10242,7 +10455,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B225" t="s">
         <v>76</v>
@@ -10254,7 +10467,7 @@
         <v>98</v>
       </c>
       <c r="E225" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F225" t="s">
         <v>120</v>
@@ -10265,7 +10478,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B226" t="s">
         <v>79</v>
@@ -10277,7 +10490,7 @@
         <v>98</v>
       </c>
       <c r="E226" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F226" t="s">
         <v>120</v>
@@ -10300,7 +10513,7 @@
         <v>98</v>
       </c>
       <c r="E227" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F227" t="s">
         <v>120</v>
@@ -10323,7 +10536,7 @@
         <v>98</v>
       </c>
       <c r="E228" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F228" t="s">
         <v>120</v>
@@ -10346,7 +10559,7 @@
         <v>98</v>
       </c>
       <c r="E229" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F229" t="s">
         <v>120</v>
@@ -10369,7 +10582,7 @@
         <v>98</v>
       </c>
       <c r="E230" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F230" t="s">
         <v>120</v>
@@ -10392,7 +10605,7 @@
         <v>98</v>
       </c>
       <c r="E231" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F231" t="s">
         <v>121</v>
@@ -10406,7 +10619,7 @@
         <v>103</v>
       </c>
       <c r="B232" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C232" t="s">
         <v>31</v>
@@ -10415,13 +10628,13 @@
         <v>98</v>
       </c>
       <c r="E232" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F232" t="s">
         <v>121</v>
       </c>
       <c r="G232" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.45">
@@ -10429,7 +10642,7 @@
         <v>103</v>
       </c>
       <c r="B233" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C233" t="s">
         <v>31</v>
@@ -10438,13 +10651,13 @@
         <v>98</v>
       </c>
       <c r="E233" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F233" t="s">
         <v>121</v>
       </c>
       <c r="G233" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.45">
@@ -10461,7 +10674,7 @@
         <v>98</v>
       </c>
       <c r="E234" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F234" t="s">
         <v>121</v>
@@ -10475,7 +10688,7 @@
         <v>103</v>
       </c>
       <c r="B235" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C235" t="s">
         <v>31</v>
@@ -10484,7 +10697,7 @@
         <v>98</v>
       </c>
       <c r="E235" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F235" t="s">
         <v>121</v>
@@ -10507,7 +10720,7 @@
         <v>98</v>
       </c>
       <c r="E236" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F236" t="s">
         <v>121</v>
@@ -10530,7 +10743,7 @@
         <v>98</v>
       </c>
       <c r="E237" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F237" t="s">
         <v>121</v>
@@ -10553,7 +10766,7 @@
         <v>98</v>
       </c>
       <c r="E238" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F238" t="s">
         <v>121</v>
@@ -10567,7 +10780,7 @@
         <v>16</v>
       </c>
       <c r="B239" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C239" t="s">
         <v>31</v>
@@ -10576,7 +10789,7 @@
         <v>98</v>
       </c>
       <c r="E239" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F239" t="s">
         <v>121</v>
@@ -10590,7 +10803,7 @@
         <v>103</v>
       </c>
       <c r="B240" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C240" t="s">
         <v>31</v>
@@ -10599,13 +10812,13 @@
         <v>98</v>
       </c>
       <c r="E240" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F240" t="s">
         <v>121</v>
       </c>
       <c r="G240" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.45">
@@ -10622,7 +10835,7 @@
         <v>98</v>
       </c>
       <c r="E241" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F241" t="s">
         <v>121</v>
@@ -10645,7 +10858,7 @@
         <v>98</v>
       </c>
       <c r="E242" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F242" t="s">
         <v>121</v>
@@ -10668,7 +10881,7 @@
         <v>98</v>
       </c>
       <c r="E243" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F243" t="s">
         <v>121</v>
@@ -10682,7 +10895,7 @@
         <v>103</v>
       </c>
       <c r="B244" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C244" t="s">
         <v>31</v>
@@ -10691,13 +10904,13 @@
         <v>98</v>
       </c>
       <c r="E244" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F244" t="s">
         <v>121</v>
       </c>
       <c r="G244" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.45">
@@ -10714,7 +10927,7 @@
         <v>98</v>
       </c>
       <c r="E245" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F245" t="s">
         <v>121</v>
@@ -10737,7 +10950,7 @@
         <v>98</v>
       </c>
       <c r="E246" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F246" t="s">
         <v>121</v>
@@ -10760,7 +10973,7 @@
         <v>98</v>
       </c>
       <c r="E247" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F247" t="s">
         <v>121</v>
@@ -10783,7 +10996,7 @@
         <v>98</v>
       </c>
       <c r="E248" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F248" t="s">
         <v>121</v>
@@ -10797,7 +11010,7 @@
         <v>71</v>
       </c>
       <c r="B249" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C249" t="s">
         <v>31</v>
@@ -10806,7 +11019,7 @@
         <v>98</v>
       </c>
       <c r="E249" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F249" t="s">
         <v>121</v>
@@ -10829,7 +11042,7 @@
         <v>98</v>
       </c>
       <c r="E250" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F250" t="s">
         <v>121</v>
@@ -10840,7 +11053,7 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B251" t="s">
         <v>17</v>
@@ -10852,7 +11065,7 @@
         <v>98</v>
       </c>
       <c r="E251" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F251" t="s">
         <v>121</v>
@@ -10875,7 +11088,7 @@
         <v>98</v>
       </c>
       <c r="E252" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F252" t="s">
         <v>121</v>
@@ -10889,7 +11102,7 @@
         <v>55</v>
       </c>
       <c r="B253" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C253" t="s">
         <v>31</v>
@@ -10898,7 +11111,7 @@
         <v>98</v>
       </c>
       <c r="E253" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F253" t="s">
         <v>121</v>
@@ -10912,7 +11125,7 @@
         <v>55</v>
       </c>
       <c r="B254" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C254" t="s">
         <v>31</v>
@@ -10921,7 +11134,7 @@
         <v>98</v>
       </c>
       <c r="E254" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F254" t="s">
         <v>121</v>
@@ -10932,7 +11145,7 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B255" t="s">
         <v>86</v>
@@ -10944,7 +11157,7 @@
         <v>98</v>
       </c>
       <c r="E255" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F255" t="s">
         <v>121</v>
@@ -10955,10 +11168,10 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B256" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C256" t="s">
         <v>31</v>
@@ -10967,13 +11180,13 @@
         <v>98</v>
       </c>
       <c r="E256" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F256" t="s">
         <v>121</v>
       </c>
       <c r="G256" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I256" t="s">
         <v>254</v>
@@ -10981,7 +11194,7 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B257" t="s">
         <v>80</v>
@@ -10993,7 +11206,7 @@
         <v>98</v>
       </c>
       <c r="E257" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F257" t="s">
         <v>121</v>
@@ -11019,7 +11232,7 @@
         <v>98</v>
       </c>
       <c r="E258" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F258" t="s">
         <v>120</v>
@@ -11042,7 +11255,7 @@
         <v>98</v>
       </c>
       <c r="E259" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F259" t="s">
         <v>120</v>
@@ -11065,7 +11278,7 @@
         <v>98</v>
       </c>
       <c r="E260" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F260" t="s">
         <v>120</v>
@@ -11088,7 +11301,7 @@
         <v>98</v>
       </c>
       <c r="E261" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F261" t="s">
         <v>120</v>
@@ -11111,7 +11324,7 @@
         <v>98</v>
       </c>
       <c r="E262" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F262" t="s">
         <v>120</v>
@@ -11134,7 +11347,7 @@
         <v>98</v>
       </c>
       <c r="E263" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F263" t="s">
         <v>120</v>
@@ -11157,7 +11370,7 @@
         <v>98</v>
       </c>
       <c r="E264" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F264" t="s">
         <v>120</v>
@@ -11180,7 +11393,7 @@
         <v>98</v>
       </c>
       <c r="E265" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F265" t="s">
         <v>120</v>
@@ -11194,7 +11407,7 @@
         <v>103</v>
       </c>
       <c r="B266" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C266" t="s">
         <v>31</v>
@@ -11203,13 +11416,13 @@
         <v>98</v>
       </c>
       <c r="E266" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F266" t="s">
         <v>120</v>
       </c>
       <c r="G266" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.45">
@@ -11226,7 +11439,7 @@
         <v>98</v>
       </c>
       <c r="E267" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F267" t="s">
         <v>120</v>
@@ -11249,7 +11462,7 @@
         <v>98</v>
       </c>
       <c r="E268" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F268" t="s">
         <v>120</v>
@@ -11272,7 +11485,7 @@
         <v>98</v>
       </c>
       <c r="E269" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F269" t="s">
         <v>120</v>
@@ -11286,7 +11499,7 @@
         <v>103</v>
       </c>
       <c r="B270" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C270" t="s">
         <v>31</v>
@@ -11295,7 +11508,7 @@
         <v>98</v>
       </c>
       <c r="E270" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F270" t="s">
         <v>120</v>
@@ -11318,7 +11531,7 @@
         <v>98</v>
       </c>
       <c r="E271" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F271" t="s">
         <v>120</v>
@@ -11341,7 +11554,7 @@
         <v>98</v>
       </c>
       <c r="E272" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F272" t="s">
         <v>120</v>
@@ -11364,7 +11577,7 @@
         <v>98</v>
       </c>
       <c r="E273" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F273" t="s">
         <v>120</v>
@@ -11387,7 +11600,7 @@
         <v>98</v>
       </c>
       <c r="E274" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F274" t="s">
         <v>120</v>
@@ -11410,7 +11623,7 @@
         <v>98</v>
       </c>
       <c r="E275" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F275" t="s">
         <v>120</v>
@@ -11433,7 +11646,7 @@
         <v>98</v>
       </c>
       <c r="E276" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F276" t="s">
         <v>120</v>
@@ -11456,7 +11669,7 @@
         <v>98</v>
       </c>
       <c r="E277" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F277" t="s">
         <v>120</v>
@@ -11479,7 +11692,7 @@
         <v>98</v>
       </c>
       <c r="E278" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F278" t="s">
         <v>120</v>
@@ -11493,7 +11706,7 @@
         <v>15</v>
       </c>
       <c r="B279" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C279" t="s">
         <v>31</v>
@@ -11502,7 +11715,7 @@
         <v>98</v>
       </c>
       <c r="E279" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F279" t="s">
         <v>120</v>
@@ -11528,7 +11741,7 @@
         <v>98</v>
       </c>
       <c r="E280" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F280" t="s">
         <v>120</v>
@@ -11551,7 +11764,7 @@
         <v>98</v>
       </c>
       <c r="E281" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F281" t="s">
         <v>120</v>
@@ -11574,7 +11787,7 @@
         <v>98</v>
       </c>
       <c r="E282" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F282" t="s">
         <v>120</v>
@@ -11597,7 +11810,7 @@
         <v>98</v>
       </c>
       <c r="E283" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F283" t="s">
         <v>120</v>
@@ -11620,7 +11833,7 @@
         <v>98</v>
       </c>
       <c r="E284" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F284" t="s">
         <v>120</v>
@@ -11643,7 +11856,7 @@
         <v>98</v>
       </c>
       <c r="E285" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F285" t="s">
         <v>120</v>
@@ -11657,7 +11870,7 @@
         <v>103</v>
       </c>
       <c r="B286" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C286" t="s">
         <v>34</v>
@@ -11666,13 +11879,13 @@
         <v>98</v>
       </c>
       <c r="E286" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F286" t="s">
         <v>120</v>
       </c>
       <c r="G286" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.45">
@@ -11689,7 +11902,7 @@
         <v>98</v>
       </c>
       <c r="E287" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F287" t="s">
         <v>120</v>
@@ -11703,7 +11916,7 @@
         <v>103</v>
       </c>
       <c r="B288" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C288" t="s">
         <v>34</v>
@@ -11712,7 +11925,7 @@
         <v>98</v>
       </c>
       <c r="E288" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F288" t="s">
         <v>120</v>
@@ -11735,7 +11948,7 @@
         <v>98</v>
       </c>
       <c r="E289" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F289" t="s">
         <v>120</v>
@@ -11749,7 +11962,7 @@
         <v>103</v>
       </c>
       <c r="B290" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C290" t="s">
         <v>34</v>
@@ -11758,13 +11971,13 @@
         <v>98</v>
       </c>
       <c r="E290" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F290" t="s">
         <v>120</v>
       </c>
       <c r="G290" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.45">
@@ -11772,7 +11985,7 @@
         <v>103</v>
       </c>
       <c r="B291" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C291" t="s">
         <v>34</v>
@@ -11781,7 +11994,7 @@
         <v>98</v>
       </c>
       <c r="E291" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F291" t="s">
         <v>120</v>
@@ -11804,7 +12017,7 @@
         <v>98</v>
       </c>
       <c r="E292" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F292" t="s">
         <v>120</v>
@@ -11827,7 +12040,7 @@
         <v>98</v>
       </c>
       <c r="E293" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F293" t="s">
         <v>120</v>
@@ -11850,7 +12063,7 @@
         <v>98</v>
       </c>
       <c r="E294" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F294" t="s">
         <v>120</v>
@@ -11873,7 +12086,7 @@
         <v>98</v>
       </c>
       <c r="E295" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F295" t="s">
         <v>120</v>
@@ -11887,7 +12100,7 @@
         <v>55</v>
       </c>
       <c r="B296" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C296" t="s">
         <v>34</v>
@@ -11896,7 +12109,7 @@
         <v>98</v>
       </c>
       <c r="E296" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F296" t="s">
         <v>120</v>
@@ -11910,7 +12123,7 @@
         <v>55</v>
       </c>
       <c r="B297" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C297" t="s">
         <v>34</v>
@@ -11919,7 +12132,7 @@
         <v>98</v>
       </c>
       <c r="E297" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F297" t="s">
         <v>120</v>
@@ -11933,7 +12146,7 @@
         <v>103</v>
       </c>
       <c r="B298" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C298" t="s">
         <v>34</v>
@@ -11942,7 +12155,7 @@
         <v>98</v>
       </c>
       <c r="E298" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F298" t="s">
         <v>120</v>
@@ -11965,7 +12178,7 @@
         <v>98</v>
       </c>
       <c r="E299" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F299" t="s">
         <v>120</v>
@@ -11979,7 +12192,7 @@
         <v>103</v>
       </c>
       <c r="B300" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C300" t="s">
         <v>34</v>
@@ -11988,7 +12201,7 @@
         <v>98</v>
       </c>
       <c r="E300" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F300" t="s">
         <v>120</v>
@@ -12011,7 +12224,7 @@
         <v>98</v>
       </c>
       <c r="E301" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F301" t="s">
         <v>120</v>
@@ -12034,7 +12247,7 @@
         <v>98</v>
       </c>
       <c r="E302" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F302" t="s">
         <v>120</v>
@@ -12048,7 +12261,7 @@
         <v>103</v>
       </c>
       <c r="B303" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C303" t="s">
         <v>34</v>
@@ -12057,7 +12270,7 @@
         <v>98</v>
       </c>
       <c r="E303" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F303" t="s">
         <v>120</v>
@@ -12080,7 +12293,7 @@
         <v>98</v>
       </c>
       <c r="E304" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F304" t="s">
         <v>120</v>
@@ -12103,7 +12316,7 @@
         <v>98</v>
       </c>
       <c r="E305" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F305" t="s">
         <v>120</v>
@@ -12126,7 +12339,7 @@
         <v>98</v>
       </c>
       <c r="E306" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F306" t="s">
         <v>120</v>
@@ -12149,7 +12362,7 @@
         <v>98</v>
       </c>
       <c r="E307" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F307" t="s">
         <v>120</v>
@@ -12172,7 +12385,7 @@
         <v>98</v>
       </c>
       <c r="E308" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F308" t="s">
         <v>120</v>
@@ -12195,7 +12408,7 @@
         <v>98</v>
       </c>
       <c r="E309" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F309" t="s">
         <v>120</v>
@@ -12218,7 +12431,7 @@
         <v>98</v>
       </c>
       <c r="E310" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F310" t="s">
         <v>120</v>
@@ -12241,7 +12454,7 @@
         <v>98</v>
       </c>
       <c r="E311" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F311" t="s">
         <v>120</v>
@@ -12264,7 +12477,7 @@
         <v>98</v>
       </c>
       <c r="E312" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F312" t="s">
         <v>120</v>
@@ -12287,7 +12500,7 @@
         <v>98</v>
       </c>
       <c r="E313" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F313" t="s">
         <v>120</v>
@@ -12301,7 +12514,7 @@
         <v>53</v>
       </c>
       <c r="B314" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C314" t="s">
         <v>34</v>
@@ -12310,7 +12523,7 @@
         <v>98</v>
       </c>
       <c r="E314" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F314" t="s">
         <v>120</v>
@@ -12333,7 +12546,7 @@
         <v>98</v>
       </c>
       <c r="E315" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F315" t="s">
         <v>120</v>
@@ -12356,7 +12569,7 @@
         <v>98</v>
       </c>
       <c r="E316" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F316" t="s">
         <v>120</v>
@@ -12370,7 +12583,7 @@
         <v>49</v>
       </c>
       <c r="B317" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C317" t="s">
         <v>34</v>
@@ -12379,7 +12592,7 @@
         <v>98</v>
       </c>
       <c r="E317" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F317" t="s">
         <v>120</v>
@@ -12393,7 +12606,7 @@
         <v>49</v>
       </c>
       <c r="B318" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C318" t="s">
         <v>34</v>
@@ -12402,7 +12615,7 @@
         <v>98</v>
       </c>
       <c r="E318" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F318" t="s">
         <v>120</v>
@@ -12416,7 +12629,7 @@
         <v>49</v>
       </c>
       <c r="B319" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C319" t="s">
         <v>34</v>
@@ -12425,7 +12638,7 @@
         <v>98</v>
       </c>
       <c r="E319" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F319" t="s">
         <v>120</v>
@@ -12448,7 +12661,7 @@
         <v>98</v>
       </c>
       <c r="E320" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F320" t="s">
         <v>120</v>
@@ -12462,7 +12675,7 @@
         <v>49</v>
       </c>
       <c r="B321" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C321" t="s">
         <v>34</v>
@@ -12471,7 +12684,7 @@
         <v>98</v>
       </c>
       <c r="E321" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F321" t="s">
         <v>120</v>
@@ -12485,7 +12698,7 @@
         <v>49</v>
       </c>
       <c r="B322" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C322" t="s">
         <v>34</v>
@@ -12494,7 +12707,7 @@
         <v>98</v>
       </c>
       <c r="E322" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F322" t="s">
         <v>120</v>
@@ -12517,7 +12730,7 @@
         <v>98</v>
       </c>
       <c r="E323" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F323" t="s">
         <v>120</v>
@@ -12540,7 +12753,7 @@
         <v>98</v>
       </c>
       <c r="E324" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F324" t="s">
         <v>120</v>
@@ -12551,7 +12764,7 @@
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B325" t="s">
         <v>61</v>
@@ -12563,7 +12776,7 @@
         <v>98</v>
       </c>
       <c r="E325" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F325" t="s">
         <v>120</v>
@@ -12586,7 +12799,7 @@
         <v>98</v>
       </c>
       <c r="E326" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F326" t="s">
         <v>120</v>
@@ -12609,7 +12822,7 @@
         <v>98</v>
       </c>
       <c r="E327" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F327" t="s">
         <v>120</v>
@@ -12632,7 +12845,7 @@
         <v>98</v>
       </c>
       <c r="E328" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F328" t="s">
         <v>120</v>
@@ -12655,7 +12868,7 @@
         <v>98</v>
       </c>
       <c r="E329" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F329" t="s">
         <v>120</v>
@@ -12678,7 +12891,7 @@
         <v>98</v>
       </c>
       <c r="E330" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F330" t="s">
         <v>120</v>
@@ -12701,7 +12914,7 @@
         <v>98</v>
       </c>
       <c r="E331" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F331" t="s">
         <v>120</v>
@@ -12807,7 +13020,7 @@
         <v>103</v>
       </c>
       <c r="B336" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C336" t="s">
         <v>34</v>
@@ -12853,7 +13066,7 @@
         <v>90</v>
       </c>
       <c r="B338" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C338" t="s">
         <v>34</v>
@@ -12873,7 +13086,7 @@
     </row>
     <row r="339" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B339" t="s">
         <v>161</v>
@@ -12899,7 +13112,7 @@
         <v>90</v>
       </c>
       <c r="B340" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C340" t="s">
         <v>34</v>
@@ -12922,7 +13135,7 @@
         <v>86</v>
       </c>
       <c r="B341" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C341" t="s">
         <v>34</v>
@@ -12942,10 +13155,10 @@
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B342" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C342" t="s">
         <v>34</v>
@@ -12968,7 +13181,7 @@
         <v>71</v>
       </c>
       <c r="B343" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C343" t="s">
         <v>34</v>
@@ -12988,10 +13201,10 @@
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B344" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C344" t="s">
         <v>34</v>
@@ -13011,10 +13224,10 @@
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B345" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C345" t="s">
         <v>34</v>
@@ -13029,7 +13242,7 @@
         <v>121</v>
       </c>
       <c r="G345" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.45">
@@ -13060,7 +13273,7 @@
         <v>205</v>
       </c>
       <c r="B347" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C347" t="s">
         <v>34</v>
@@ -13083,7 +13296,7 @@
         <v>71</v>
       </c>
       <c r="B348" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C348" t="s">
         <v>34</v>
@@ -13103,10 +13316,10 @@
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B349" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C349" t="s">
         <v>34</v>
@@ -13152,7 +13365,7 @@
         <v>91</v>
       </c>
       <c r="B351" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C351" t="s">
         <v>34</v>
@@ -13172,10 +13385,10 @@
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B352" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C352" t="s">
         <v>34</v>
@@ -13190,7 +13403,7 @@
         <v>121</v>
       </c>
       <c r="G352" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.45">
@@ -13198,7 +13411,7 @@
         <v>228</v>
       </c>
       <c r="B353" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C353" t="s">
         <v>34</v>
@@ -13221,7 +13434,7 @@
         <v>228</v>
       </c>
       <c r="B354" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C354" t="s">
         <v>34</v>
@@ -13267,7 +13480,7 @@
         <v>221</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -13281,7 +13494,7 @@
         <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -13295,7 +13508,7 @@
         <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -13309,7 +13522,7 @@
         <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -13323,7 +13536,7 @@
         <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -13337,7 +13550,7 @@
         <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -13351,7 +13564,7 @@
         <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -13365,7 +13578,7 @@
         <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -13379,96 +13592,96 @@
         <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C10" t="s">
         <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C11" t="s">
         <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C12" t="s">
         <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C13" t="s">
         <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C14" t="s">
         <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C15" t="s">
         <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B16" t="s">
         <v>189</v>
@@ -13477,21 +13690,21 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C17" t="s">
         <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>